<commit_message>
Fixed component orientation in CPL file.
</commit_message>
<xml_diff>
--- a/v0p2/gerber_v0p2_r1/CPL_JLCPCB.xlsx
+++ b/v0p2/gerber_v0p2_r1/CPL_JLCPCB.xlsx
@@ -208,7 +208,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -407,7 +407,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>